<commit_message>
Add questionnaire for phase 1
</commit_message>
<xml_diff>
--- a/Phase-I.xlsx
+++ b/Phase-I.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Heena\Desktop\Back_up\PhD_Monika\InfosysInternship\BPQual\Relevant\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Heena\Documents\GitHub\QualitativeStudy\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,7 +15,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$F$1:$F$130</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$E$1:$E$130</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -27,15 +27,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="306">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="305">
   <si>
     <t>Resposne ID</t>
   </si>
   <si>
     <t xml:space="preserve">Problem </t>
-  </si>
-  <si>
-    <t>Category</t>
   </si>
   <si>
     <t xml:space="preserve">Experience </t>
@@ -927,9 +924,6 @@
     <t>Increased accuracy of production systems -&gt; increase in Compliance -&gt; Reduced manual efforts employed for sampling.</t>
   </si>
   <si>
-    <t>Descriptor</t>
-  </si>
-  <si>
     <t>C1, C2</t>
   </si>
   <si>
@@ -1066,6 +1060,9 @@
   </si>
   <si>
     <t>Survey followed by in-person discussion</t>
+  </si>
+  <si>
+    <t>Problem Statement</t>
   </si>
 </sst>
 </file>
@@ -1472,26 +1469,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I130"/>
+  <dimension ref="A1:H130"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="D103" sqref="D103:D108"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.85546875" style="5" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="43.5703125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="27.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.85546875" style="5" customWidth="1"/>
-    <col min="8" max="8" width="30.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" style="5" customWidth="1"/>
+    <col min="7" max="7" width="30.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.5703125" style="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>259</v>
+        <v>304</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>0</v>
@@ -1500,2254 +1497,2250 @@
         <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>2</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>5</v>
       </c>
       <c r="G1" s="4" t="s">
         <v>3</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="B2" s="5">
         <v>9</v>
       </c>
       <c r="C2" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="B3" s="5">
         <v>27</v>
       </c>
       <c r="C3" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="B4" s="5">
         <v>41</v>
       </c>
       <c r="C4" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>223</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="B5" s="5">
         <v>43</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="120" x14ac:dyDescent="0.25">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="B6" s="5">
         <v>1</v>
       </c>
       <c r="C6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="E6" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F6" s="5" t="s">
-        <v>9</v>
+      <c r="F6" s="5">
+        <v>11</v>
       </c>
       <c r="G6" s="5">
-        <v>11</v>
-      </c>
-      <c r="H6" s="5">
         <v>2</v>
       </c>
-      <c r="I6" s="6" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="H6" s="6" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B7" s="5">
         <v>5</v>
       </c>
       <c r="C7" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="E7" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="F7" s="5" t="s">
-        <v>32</v>
+      <c r="F7" s="5">
+        <v>10</v>
       </c>
       <c r="G7" s="5">
-        <v>10</v>
-      </c>
-      <c r="H7" s="5">
         <v>1</v>
       </c>
-      <c r="I7" s="6" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="H7" s="6" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B8" s="5">
         <v>22</v>
       </c>
       <c r="C8" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="D8" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="D8" s="3" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B9" s="5">
         <v>38</v>
       </c>
       <c r="C9" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>201</v>
       </c>
-      <c r="D9" s="3" t="s">
-        <v>202</v>
-      </c>
-      <c r="I9" s="6" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="H9" s="6" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B10" s="5">
         <v>8</v>
       </c>
       <c r="C10" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D10" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="D10" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>9</v>
+      <c r="E10" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F10" s="5">
+        <v>12</v>
       </c>
       <c r="G10" s="5">
-        <v>12</v>
-      </c>
-      <c r="H10" s="5">
         <v>4</v>
       </c>
-      <c r="I10" s="6" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="H10" s="6" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B11" s="5">
         <v>11</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B12" s="5">
         <v>13</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B13" s="5">
         <v>16</v>
       </c>
       <c r="C13" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="D13" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="D13" s="3" t="s">
-        <v>86</v>
+      <c r="E13" s="5" t="s">
+        <v>81</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="H13" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="I13" s="6" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B14" s="5">
         <v>39</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="B15" s="5">
         <v>9</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="F15" s="5" t="s">
         <v>48</v>
       </c>
+      <c r="E15" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="F15" s="5">
+        <v>16</v>
+      </c>
       <c r="G15" s="5">
-        <v>16</v>
-      </c>
-      <c r="H15" s="5">
         <v>14</v>
       </c>
-      <c r="I15" s="6" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="H15" s="6" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B16" s="5">
         <v>8</v>
       </c>
       <c r="C16" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D16" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="D16" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B17" s="5">
         <v>14</v>
       </c>
       <c r="C17" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="E17" s="5" t="s">
         <v>81</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="H17" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="I17" s="6" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+      <c r="H17" s="6" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B18" s="5">
         <v>18</v>
       </c>
       <c r="C18" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="D18" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="D18" s="3" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B19" s="5">
         <v>27</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B20" s="5">
         <v>32</v>
       </c>
       <c r="C20" s="14" t="s">
+        <v>174</v>
+      </c>
+      <c r="D20" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="D20" s="3" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B21" s="5">
         <v>43</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B22" s="5">
         <v>2</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B23" s="5">
         <v>6</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="F23" s="5" t="s">
-        <v>38</v>
+        <v>34</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="F23" s="5">
+        <v>9</v>
       </c>
       <c r="G23" s="5">
-        <v>9</v>
-      </c>
-      <c r="H23" s="5">
         <v>2</v>
       </c>
-      <c r="I23" s="6" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="H23" s="6" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="B24" s="5">
         <v>10</v>
       </c>
       <c r="C24" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D24" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="D24" s="3" t="s">
+      <c r="E24" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="F24" s="5" t="s">
-        <v>54</v>
+      <c r="F24" s="5">
+        <v>12</v>
       </c>
       <c r="G24" s="5">
-        <v>12</v>
-      </c>
-      <c r="H24" s="5">
         <v>6</v>
       </c>
-      <c r="I24" s="6" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="H24" s="6" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="B25" s="5">
         <v>11</v>
       </c>
       <c r="C25" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D25" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="D25" s="3" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B26" s="5">
         <v>15</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="B27" s="5">
         <v>19</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>297</v>
+        <v>295</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>81</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="H27" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="I27" s="6" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+      <c r="H27" s="6" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="B28" s="5">
         <v>45</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>81</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G28" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="H28" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="I28" s="6" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+      <c r="H28" s="6" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="B29" s="5">
         <v>34</v>
       </c>
       <c r="C29" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="D29" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="D29" s="3" t="s">
-        <v>180</v>
-      </c>
-      <c r="F29" s="5" t="s">
-        <v>185</v>
+      <c r="E29" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="F29" s="5">
+        <v>17</v>
       </c>
       <c r="G29" s="5">
-        <v>17</v>
-      </c>
-      <c r="H29" s="5">
         <v>4</v>
       </c>
-      <c r="I29" s="6" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="H29" s="6" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B30" s="5">
         <v>11</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="B31" s="5">
         <v>13</v>
       </c>
       <c r="C31" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D31" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="D31" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="F31" s="5" t="s">
-        <v>68</v>
+      <c r="E31" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="F31" s="5">
+        <v>17</v>
       </c>
       <c r="G31" s="5">
-        <v>17</v>
-      </c>
-      <c r="H31" s="5">
         <v>14</v>
       </c>
-      <c r="I31" s="6" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" s="16" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="H31" s="6" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" s="16" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A32" s="16" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="B32" s="17">
         <v>35</v>
       </c>
       <c r="C32" s="18" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D32" s="18"/>
+      <c r="E32" s="17"/>
       <c r="F32" s="17"/>
       <c r="G32" s="17"/>
-      <c r="H32" s="17"/>
-      <c r="I32" s="20"/>
-    </row>
-    <row r="33" spans="1:9" s="10" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="H32" s="20"/>
+    </row>
+    <row r="33" spans="1:8" s="10" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A33" s="10" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="B33" s="19">
         <v>17</v>
       </c>
       <c r="C33" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="D33" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="D33" s="14" t="s">
-        <v>94</v>
-      </c>
+      <c r="E33" s="19"/>
       <c r="F33" s="19"/>
       <c r="G33" s="19"/>
-      <c r="H33" s="19"/>
-      <c r="I33" s="21"/>
-    </row>
-    <row r="34" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+      <c r="H33" s="21"/>
+    </row>
+    <row r="34" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B34" s="5">
         <v>26</v>
       </c>
       <c r="C34" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="D34" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="D34" s="3" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="B35" s="5">
         <v>14</v>
       </c>
       <c r="C35" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="D35" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="D35" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="B36" s="5">
         <v>43</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="B37" s="5">
         <v>16</v>
       </c>
       <c r="C37" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D37" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="D37" s="3" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B38" s="5">
         <v>3</v>
       </c>
       <c r="C38" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D38" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D38" s="3" t="s">
+      <c r="E38" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F38" s="5" t="s">
-        <v>20</v>
+      <c r="F38" s="5">
+        <v>10</v>
       </c>
       <c r="G38" s="5">
-        <v>10</v>
-      </c>
-      <c r="H38" s="5">
         <v>7</v>
       </c>
     </row>
-    <row r="39" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="B39" s="5">
         <v>10</v>
       </c>
       <c r="C39" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D39" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="D39" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B40" s="5">
         <v>14</v>
       </c>
       <c r="C40" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D40" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="D40" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="F40" s="5" t="s">
-        <v>76</v>
+      <c r="E40" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="F40" s="5">
+        <v>21</v>
       </c>
       <c r="G40" s="5">
-        <v>21</v>
-      </c>
-      <c r="H40" s="5">
         <v>10</v>
       </c>
-      <c r="I40" s="6" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="H40" s="6" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B41" s="5">
         <v>19</v>
       </c>
       <c r="C41" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="D41" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="D41" s="3" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" ht="39" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" spans="1:8" ht="39" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B42" s="5">
         <v>46</v>
       </c>
       <c r="C42" s="12" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D42" s="12" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B43" s="5">
         <v>20</v>
       </c>
       <c r="C43" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="D43" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="D43" s="3" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="44" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="B44" s="5">
         <v>19</v>
       </c>
       <c r="C44" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="D44" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="D44" s="3" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="45" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="B45" s="5">
         <v>20</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="F45" s="5" t="s">
-        <v>9</v>
+        <v>105</v>
+      </c>
+      <c r="E45" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F45" s="5">
+        <v>11</v>
       </c>
       <c r="G45" s="5">
-        <v>11</v>
-      </c>
-      <c r="H45" s="5">
         <v>2</v>
       </c>
     </row>
-    <row r="46" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="B46" s="5">
         <v>22</v>
       </c>
       <c r="C46" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="D46" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="D46" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="F46" s="5" t="s">
-        <v>120</v>
+      <c r="E46" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="F46" s="5">
+        <v>15</v>
       </c>
       <c r="G46" s="5">
-        <v>15</v>
-      </c>
-      <c r="H46" s="5">
         <v>5</v>
       </c>
-      <c r="I46" s="6" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="H46" s="6" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="B47" s="5">
         <v>34</v>
       </c>
       <c r="C47" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="D47" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="D47" s="3" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="48" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="B48" s="5">
         <v>38</v>
       </c>
       <c r="C48" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="D48" s="3" t="s">
         <v>203</v>
       </c>
-      <c r="D48" s="3" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="49" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="B49" s="5">
         <v>38</v>
       </c>
       <c r="C49" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="D49" s="3" t="s">
         <v>210</v>
       </c>
-      <c r="D49" s="3" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+    </row>
+    <row r="50" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="B50" s="5">
         <v>20</v>
       </c>
       <c r="C50" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="D50" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="D50" s="3" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="51" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="6" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="B51" s="5">
         <v>24</v>
       </c>
       <c r="C51" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="D51" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="D51" s="3" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    </row>
+    <row r="52" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A52" s="6" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="B52" s="5">
         <v>25</v>
       </c>
       <c r="C52" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="D52" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="D52" s="3" t="s">
+      <c r="E52" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="F52" s="5" t="s">
-        <v>139</v>
+      <c r="F52" s="5">
+        <v>18</v>
       </c>
       <c r="G52" s="5">
-        <v>18</v>
-      </c>
-      <c r="H52" s="5">
         <v>14</v>
       </c>
-      <c r="I52" s="6" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="H52" s="6" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="B53" s="5">
         <v>35</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="B54" s="5">
         <v>41</v>
       </c>
       <c r="C54" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="D54" s="3" t="s">
         <v>225</v>
       </c>
-      <c r="D54" s="3" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    </row>
+    <row r="55" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="B55" s="5">
         <v>43</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" s="15" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" s="15" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A56" s="15" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="B56" s="4">
         <v>44</v>
       </c>
       <c r="C56" s="15" t="s">
+        <v>249</v>
+      </c>
+      <c r="D56" s="7" t="s">
         <v>250</v>
       </c>
-      <c r="D56" s="7" t="s">
-        <v>251</v>
-      </c>
+      <c r="E56" s="4"/>
       <c r="F56" s="4"/>
       <c r="G56" s="4"/>
-      <c r="H56" s="4"/>
-      <c r="I56" s="22"/>
-    </row>
-    <row r="57" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="H56" s="22"/>
+    </row>
+    <row r="57" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A57" s="6" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B57" s="5">
         <v>24</v>
       </c>
       <c r="C57" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="D57" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="D57" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="F57" s="5" t="s">
-        <v>136</v>
+      <c r="E57" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="F57" s="5">
+        <v>15</v>
       </c>
       <c r="G57" s="5">
-        <v>15</v>
-      </c>
-      <c r="H57" s="5">
         <v>10</v>
       </c>
-      <c r="I57" s="6" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="H57" s="6" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A58" s="6" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="B58" s="5">
         <v>23</v>
       </c>
       <c r="C58" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="D58" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="D58" s="3" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="59" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B59" s="5">
         <v>27</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="F59" s="5" t="s">
-        <v>9</v>
+        <v>152</v>
+      </c>
+      <c r="E59" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F59" s="5">
+        <v>10</v>
       </c>
       <c r="G59" s="5">
-        <v>10</v>
-      </c>
-      <c r="H59" s="5">
         <v>2</v>
       </c>
-      <c r="I59" s="6" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="H59" s="6" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B60" s="5">
         <v>35</v>
       </c>
       <c r="C60" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="E60" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="F60" s="5">
+        <v>14</v>
+      </c>
+      <c r="G60" s="5" t="s">
         <v>186</v>
       </c>
-      <c r="F60" s="5" t="s">
-        <v>170</v>
-      </c>
-      <c r="G60" s="5">
-        <v>14</v>
-      </c>
-      <c r="H60" s="5" t="s">
-        <v>187</v>
-      </c>
-      <c r="I60" s="6" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="H60" s="6" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="B61" s="5">
         <v>29</v>
       </c>
       <c r="C61" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="D61" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="D61" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="F61" s="5" t="s">
-        <v>9</v>
+      <c r="E61" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F61" s="5">
+        <v>11</v>
       </c>
       <c r="G61" s="5">
-        <v>11</v>
-      </c>
-      <c r="H61" s="5">
         <v>2</v>
       </c>
-      <c r="I61" s="6" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="62" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+      <c r="H61" s="6" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="B62" s="5">
         <v>40</v>
       </c>
       <c r="C62" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="D62" s="3" t="s">
         <v>219</v>
       </c>
-      <c r="D62" s="3" t="s">
-        <v>220</v>
-      </c>
-      <c r="F62" s="5" t="s">
-        <v>215</v>
+      <c r="E62" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="F62" s="5">
+        <v>18</v>
       </c>
       <c r="G62" s="5">
-        <v>18</v>
-      </c>
-      <c r="H62" s="5">
         <v>12</v>
       </c>
-      <c r="I62" s="6" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="H62" s="6" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B63" s="5">
         <v>29</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B64" s="5">
         <v>31</v>
       </c>
       <c r="C64" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="D64" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="D64" s="3" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="65" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="65" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B65" s="5">
         <v>43</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>238</v>
+        <v>237</v>
+      </c>
+      <c r="E65" s="5" t="s">
+        <v>81</v>
       </c>
       <c r="F65" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G65" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="H65" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="I65" s="6" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="66" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+      <c r="H65" s="6" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="B66" s="5">
         <v>2</v>
       </c>
       <c r="C66" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D66" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E66" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D66" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F66" s="5" t="s">
-        <v>12</v>
+      <c r="F66" s="5">
+        <v>8</v>
       </c>
       <c r="G66" s="5">
-        <v>8</v>
-      </c>
-      <c r="H66" s="5">
         <v>2.5</v>
       </c>
-      <c r="I66" s="6" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="67" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="H66" s="6" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="B67" s="5">
         <v>30</v>
       </c>
       <c r="C67" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="D67" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="D67" s="3" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="68" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    </row>
+    <row r="68" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="B68" s="5">
         <v>44</v>
       </c>
       <c r="C68" s="8" t="s">
+        <v>247</v>
+      </c>
+      <c r="D68" s="9" t="s">
         <v>248</v>
       </c>
-      <c r="D68" s="9" t="s">
-        <v>249</v>
-      </c>
-      <c r="E68" s="10"/>
-      <c r="F68" s="11" t="s">
-        <v>247</v>
+      <c r="E68" s="11" t="s">
+        <v>246</v>
+      </c>
+      <c r="F68" s="5">
+        <v>11</v>
       </c>
       <c r="G68" s="5">
-        <v>11</v>
-      </c>
-      <c r="H68" s="5">
         <v>5</v>
       </c>
-      <c r="I68" s="6" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="69" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="H68" s="6" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="B69" s="5">
         <v>34</v>
       </c>
       <c r="C69" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="D69" s="3" t="s">
         <v>181</v>
       </c>
-      <c r="D69" s="3" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="70" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="70" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B70" s="5">
         <v>2</v>
       </c>
       <c r="C70" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D70" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D70" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="71" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="71" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B71" s="5">
         <v>6</v>
       </c>
       <c r="C71" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D71" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D71" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="72" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    </row>
+    <row r="72" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B72" s="5">
         <v>11</v>
       </c>
       <c r="C72" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D72" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="D72" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="F72" s="5" t="s">
-        <v>23</v>
+      <c r="E72" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F72" s="5">
+        <v>13</v>
       </c>
       <c r="G72" s="5">
-        <v>13</v>
-      </c>
-      <c r="H72" s="5">
         <v>6</v>
       </c>
-      <c r="I72" s="6" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="73" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+      <c r="H72" s="6" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B73" s="5">
         <v>23</v>
       </c>
       <c r="C73" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="D73" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="D73" s="3" t="s">
+      <c r="E73" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="F73" s="5" t="s">
-        <v>125</v>
+      <c r="F73" s="5">
+        <v>9</v>
       </c>
       <c r="G73" s="5">
-        <v>9</v>
-      </c>
-      <c r="H73" s="5">
         <v>5</v>
       </c>
-      <c r="I73" s="6" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="74" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="H73" s="6" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B74" s="5">
         <v>25</v>
       </c>
       <c r="C74" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="D74" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="D74" s="3" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="75" spans="1:9" ht="51" x14ac:dyDescent="0.25">
+    </row>
+    <row r="75" spans="1:8" ht="51" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B75" s="5">
         <v>46</v>
       </c>
       <c r="C75" s="13" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D75" s="12" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="76" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B76" s="5">
         <v>13</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D76" s="3" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="77" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B77" s="5">
         <v>2</v>
       </c>
       <c r="C77" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D77" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D77" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B78" s="5">
         <v>30</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D78" s="3" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="79" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B79" s="5">
         <v>4</v>
       </c>
       <c r="C79" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D79" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D79" s="3" t="s">
+      <c r="E79" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="F79" s="5" t="s">
-        <v>23</v>
+      <c r="F79" s="5">
+        <v>11</v>
       </c>
       <c r="G79" s="5">
-        <v>11</v>
-      </c>
-      <c r="H79" s="5">
         <v>4.5</v>
       </c>
-      <c r="I79" s="6" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="80" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="H79" s="6" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B80" s="5">
         <v>11</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="D80" s="3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="81" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B81" s="5">
         <v>26</v>
       </c>
       <c r="C81" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="D81" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="D81" s="3" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="82" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="82" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B82" s="5">
         <v>38</v>
       </c>
       <c r="C82" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="D82" s="3" t="s">
         <v>206</v>
       </c>
-      <c r="D82" s="3" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="83" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="83" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B83" s="5">
         <v>39</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="D83" s="3" t="s">
-        <v>212</v>
-      </c>
-      <c r="F83" s="5" t="s">
-        <v>215</v>
+        <v>211</v>
+      </c>
+      <c r="E83" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="F83" s="5">
+        <v>20</v>
       </c>
       <c r="G83" s="5">
-        <v>20</v>
-      </c>
-      <c r="H83" s="5">
         <v>10</v>
       </c>
-      <c r="I83" s="6" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="84" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="H83" s="6" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B84" s="5">
         <v>42</v>
       </c>
       <c r="C84" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="D84" s="3" t="s">
         <v>236</v>
       </c>
-      <c r="D84" s="3" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="85" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="85" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B85" s="5">
         <v>10</v>
       </c>
       <c r="C85" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D85" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="86" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B86" s="5">
         <v>5</v>
       </c>
       <c r="C86" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D86" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D86" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="87" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="87" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B87" s="5">
         <v>33</v>
       </c>
       <c r="C87" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="E87" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="F87" s="3" t="s">
-        <v>178</v>
+      <c r="F87" s="5">
+        <v>15</v>
       </c>
       <c r="G87" s="5">
-        <v>15</v>
-      </c>
-      <c r="H87" s="5">
         <v>3</v>
       </c>
-      <c r="I87" s="6" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="88" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="H87" s="6" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B88" s="5">
         <v>36</v>
       </c>
       <c r="C88" s="3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D88" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="F88" s="5" t="s">
-        <v>170</v>
+        <v>191</v>
+      </c>
+      <c r="E88" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="F88" s="5">
+        <v>13</v>
       </c>
       <c r="G88" s="5">
-        <v>13</v>
-      </c>
-      <c r="H88" s="5">
         <v>3</v>
       </c>
-      <c r="I88" s="6" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="89" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="H88" s="6" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B89" s="5">
         <v>41</v>
       </c>
       <c r="C89" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="D89" s="3" t="s">
         <v>229</v>
       </c>
-      <c r="D89" s="3" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="90" spans="1:9" ht="240" x14ac:dyDescent="0.25">
+    </row>
+    <row r="90" spans="1:8" ht="240" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B90" s="5">
         <v>18</v>
       </c>
       <c r="C90" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D90" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="D90" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="F90" s="5" t="s">
-        <v>95</v>
+      <c r="E90" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="F90" s="5">
+        <v>18</v>
       </c>
       <c r="G90" s="5">
-        <v>18</v>
-      </c>
-      <c r="H90" s="5">
         <v>14</v>
       </c>
     </row>
-    <row r="91" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B91" s="5">
         <v>7</v>
       </c>
       <c r="C91" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D91" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="D91" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="F91" s="5" t="s">
-        <v>41</v>
+      <c r="E91" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="F91" s="5">
+        <v>9</v>
       </c>
       <c r="G91" s="5">
-        <v>9</v>
-      </c>
-      <c r="H91" s="5">
         <v>1</v>
       </c>
-      <c r="I91" s="6" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="92" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="H91" s="6" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B92" s="5">
         <v>11</v>
       </c>
       <c r="C92" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D92" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="D92" s="3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="93" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="93" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B93" s="5">
         <v>15</v>
       </c>
       <c r="C93" s="3" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="94" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A94" s="6" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B94" s="5">
         <v>23</v>
       </c>
       <c r="C94" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="D94" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="D94" s="3" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="95" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    </row>
+    <row r="95" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A95" s="5" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B95" s="5">
         <v>24</v>
       </c>
       <c r="C95" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="D95" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="D95" s="3" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="96" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="96" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B96" s="5">
         <v>30</v>
       </c>
       <c r="C96" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="D96" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="D96" s="3" t="s">
-        <v>165</v>
-      </c>
-      <c r="F96" s="5" t="s">
-        <v>170</v>
+      <c r="E96" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="F96" s="5">
+        <v>12</v>
       </c>
       <c r="G96" s="5">
-        <v>12</v>
-      </c>
-      <c r="H96" s="5">
         <v>3</v>
       </c>
-      <c r="I96" s="6" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="97" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="H96" s="6" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B97" s="5">
         <v>37</v>
       </c>
       <c r="C97" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="D97" s="3" t="s">
         <v>196</v>
       </c>
-      <c r="D97" s="3" t="s">
+      <c r="E97" s="5" t="s">
         <v>197</v>
       </c>
-      <c r="F97" s="5" t="s">
-        <v>198</v>
+      <c r="F97" s="5">
+        <v>14</v>
       </c>
       <c r="G97" s="5">
-        <v>14</v>
-      </c>
-      <c r="H97" s="5">
         <v>7</v>
       </c>
-      <c r="I97" s="6" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="98" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="H97" s="6" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B98" s="5">
         <v>37</v>
       </c>
       <c r="C98" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D98" s="3" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="99" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B99" s="5">
         <v>38</v>
       </c>
       <c r="C99" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="D99" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="D99" s="3" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B100" s="5">
         <v>41</v>
       </c>
       <c r="C100" s="3" t="s">
+        <v>226</v>
+      </c>
+      <c r="D100" s="3" t="s">
         <v>227</v>
       </c>
-      <c r="D100" s="3" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="101" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="101" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B101" s="5">
         <v>43</v>
       </c>
       <c r="C101" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="D101" s="3" t="s">
         <v>244</v>
       </c>
-      <c r="D101" s="3" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="102" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    </row>
+    <row r="102" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B102" s="5">
         <v>45</v>
       </c>
       <c r="C102" s="3" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="103" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B103" s="5">
         <v>4</v>
       </c>
       <c r="C103" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D103" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="104" spans="1:9" ht="120" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B104" s="5">
         <v>17</v>
       </c>
       <c r="C104" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="D104" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="D104" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="F104" s="5" t="s">
-        <v>9</v>
+      <c r="E104" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F104" s="5">
+        <v>11</v>
       </c>
       <c r="G104" s="5">
-        <v>11</v>
-      </c>
-      <c r="H104" s="5">
         <v>4</v>
       </c>
-      <c r="I104" s="6" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="105" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="H104" s="6" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B105" s="5">
         <v>26</v>
       </c>
       <c r="C105" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="D105" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="D105" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="F105" s="5" t="s">
-        <v>148</v>
+      <c r="E105" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="F105" s="5">
+        <v>12</v>
       </c>
       <c r="G105" s="5">
-        <v>12</v>
-      </c>
-      <c r="H105" s="5">
         <v>8</v>
       </c>
-      <c r="I105" s="6" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H105" s="6" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B106" s="5">
         <v>36</v>
       </c>
       <c r="C106" s="3" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="107" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B107" s="5">
         <v>41</v>
       </c>
       <c r="C107" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="D107" s="3" t="s">
         <v>221</v>
       </c>
-      <c r="D107" s="3" t="s">
-        <v>222</v>
-      </c>
-      <c r="F107" s="5" t="s">
-        <v>218</v>
+      <c r="E107" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="F107" s="5">
+        <v>14</v>
       </c>
       <c r="G107" s="5">
-        <v>14</v>
-      </c>
-      <c r="H107" s="5">
         <v>10</v>
       </c>
-      <c r="I107" s="6" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="108" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="H107" s="6" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B108" s="5">
         <v>42</v>
       </c>
       <c r="C108" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="D108" s="3" t="s">
         <v>234</v>
       </c>
-      <c r="D108" s="3" t="s">
-        <v>235</v>
-      </c>
-      <c r="F108" s="5" t="s">
-        <v>233</v>
+      <c r="E108" s="5" t="s">
+        <v>232</v>
+      </c>
+      <c r="F108" s="5">
+        <v>18</v>
       </c>
       <c r="G108" s="5">
-        <v>18</v>
-      </c>
-      <c r="H108" s="5">
         <v>10</v>
       </c>
-      <c r="I108" s="6" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="109" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="H108" s="6" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="B109" s="5">
         <v>43</v>
       </c>
       <c r="C109" s="3" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="110" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="110" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B110" s="5">
         <v>45</v>
       </c>
       <c r="C110" s="3" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="111" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B111" s="5">
         <v>4</v>
       </c>
       <c r="C111" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D111" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D111" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B112" s="5">
         <v>7</v>
       </c>
       <c r="C112" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D112" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D112" s="3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B113" s="5">
         <v>12</v>
       </c>
       <c r="C113" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="I113" s="6" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="114" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+      <c r="H113" s="6" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="114" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B114" s="5">
         <v>17</v>
       </c>
       <c r="C114" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D114" s="3" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="115" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="115" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B115" s="5">
         <v>18</v>
       </c>
       <c r="C115" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="D115" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="D115" s="3" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="116" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="116" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="B116" s="5">
         <v>20</v>
       </c>
       <c r="C116" s="3" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="117" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="117" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B117" s="5">
         <v>21</v>
       </c>
       <c r="C117" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D117" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="F117" s="5" t="s">
-        <v>95</v>
+        <v>110</v>
+      </c>
+      <c r="E117" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="F117" s="5">
+        <v>17</v>
       </c>
       <c r="G117" s="5">
-        <v>17</v>
-      </c>
-      <c r="H117" s="5">
         <v>12</v>
       </c>
     </row>
-    <row r="118" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B118" s="5">
         <v>21</v>
       </c>
       <c r="C118" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D118" s="3" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="119" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="119" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B119" s="5">
         <v>21</v>
       </c>
       <c r="C119" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="D119" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="D119" s="3" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B120" s="5">
         <v>22</v>
       </c>
       <c r="C120" s="3" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="121" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="121" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="B121" s="5">
         <v>25</v>
       </c>
       <c r="C121" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="D121" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="D121" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="122" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    </row>
+    <row r="122" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B122" s="5">
         <v>27</v>
       </c>
       <c r="C122" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="D122" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="D122" s="3" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="123" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    </row>
+    <row r="123" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B123" s="5">
         <v>28</v>
       </c>
       <c r="C123" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="D123" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="D123" s="3" t="s">
+      <c r="E123" s="5" t="s">
         <v>159</v>
       </c>
-      <c r="F123" s="5" t="s">
-        <v>160</v>
+      <c r="F123" s="5">
+        <v>17</v>
       </c>
       <c r="G123" s="5">
-        <v>17</v>
-      </c>
-      <c r="H123" s="5">
         <v>10</v>
       </c>
-      <c r="I123" s="6" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H123" s="6" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B124" s="5">
         <v>31</v>
       </c>
       <c r="C124" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="E124" s="5" t="s">
         <v>171</v>
       </c>
-      <c r="F124" s="5" t="s">
-        <v>172</v>
+      <c r="F124" s="5">
+        <v>14</v>
       </c>
       <c r="G124" s="5">
-        <v>14</v>
-      </c>
-      <c r="H124" s="5">
         <v>6</v>
       </c>
-      <c r="I124" s="6" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H124" s="6" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B125" s="5">
         <v>36</v>
       </c>
       <c r="C125" s="3" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B126" s="5">
         <v>36</v>
       </c>
       <c r="C126" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="D126" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="D126" s="3" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="127" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="127" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B127" s="5">
         <v>37</v>
       </c>
       <c r="C127" s="3" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B128" s="5">
         <v>39</v>
       </c>
       <c r="C128" s="3" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="129" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B129" s="5">
         <v>39</v>
       </c>
       <c r="C129" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="D129" s="3" t="s">
         <v>216</v>
-      </c>
-      <c r="D129" s="3" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="130" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B130" s="5">
         <v>41</v>
       </c>
       <c r="C130" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="D130" s="3" t="s">
         <v>231</v>
       </c>
-      <c r="D130" s="3" t="s">
-        <v>232</v>
-      </c>
     </row>
   </sheetData>
-  <autoFilter ref="F1:F130"/>
+  <autoFilter ref="E1:E130"/>
   <sortState ref="A2:I130">
     <sortCondition ref="A2:A130"/>
   </sortState>

</xml_diff>